<commit_message>
adattati messaggi a nuove specifiche
</commit_message>
<xml_diff>
--- a/CensimentoEnti.xlsx
+++ b/CensimentoEnti.xlsx
@@ -445,7 +445,7 @@
         <v>Postman Sun Mock Service</v>
       </c>
       <c r="G2" t="str">
-        <v xml:space="preserve">Postman Hospital 1 </v>
+        <v xml:space="preserve">NEW Postman Hospital 1 </v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         <v>Postman Sky Mock Service</v>
       </c>
       <c r="G3" t="str">
-        <v>Postman Hospital 2</v>
+        <v>NEW Postman Hospital 2</v>
       </c>
     </row>
     <row r="4">
@@ -491,7 +491,7 @@
         <v>Postman Moon Mock Service</v>
       </c>
       <c r="G4" t="str">
-        <v>Postman Hospital 3</v>
+        <v>NEW Postman Hospital 3</v>
       </c>
     </row>
     <row r="5">
@@ -514,7 +514,7 @@
         <v>Postman Milky Mock Service</v>
       </c>
       <c r="G5" t="str">
-        <v>Postman Hospital 4</v>
+        <v>NEW Postman Hospital 4</v>
       </c>
     </row>
     <row r="6">
@@ -537,7 +537,7 @@
         <v>Postman Star Mock Service</v>
       </c>
       <c r="G6" t="str">
-        <v>Postman Hospital 5</v>
+        <v>NEW Postman Hospital 5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the bug that was preventing the extraction of codes with leading zeros
</commit_message>
<xml_diff>
--- a/CensimentoEnti.xlsx
+++ b/CensimentoEnti.xlsx
@@ -1,41 +1,152 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.dileo\Documents\Python3\PostmanHospital\Postman-Hospital-Py\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED0F66-1665-4488-AE09-8975E82C40B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+  <si>
+    <t>Ospedale</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Codice L1</t>
+  </si>
+  <si>
+    <t>Codice L2</t>
+  </si>
+  <si>
+    <t>Codice Applicativo</t>
+  </si>
+  <si>
+    <t>Nome applicativo</t>
+  </si>
+  <si>
+    <t>Nome Collection Postman</t>
+  </si>
+  <si>
+    <t>Postman Space Hospital</t>
+  </si>
+  <si>
+    <t>Comet Lab</t>
+  </si>
+  <si>
+    <t>309672</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Postman Sun Mock Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW Postman Hospital 1 </t>
+  </si>
+  <si>
+    <t>Nova Lab</t>
+  </si>
+  <si>
+    <t>0912</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Postman Sky Mock Service</t>
+  </si>
+  <si>
+    <t>NEW Postman Hospital 2</t>
+  </si>
+  <si>
+    <t>Postman Galaxy Hospital</t>
+  </si>
+  <si>
+    <t>Orbit Lab</t>
+  </si>
+  <si>
+    <t>462801</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Postman Moon Mock Service</t>
+  </si>
+  <si>
+    <t>NEW Postman Hospital 3</t>
+  </si>
+  <si>
+    <t>Nebula Lab</t>
+  </si>
+  <si>
+    <t>5678</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Postman Milky Mock Service</t>
+  </si>
+  <si>
+    <t>NEW Postman Hospital 4</t>
+  </si>
+  <si>
+    <t>Postman Cosmo Hospital</t>
+  </si>
+  <si>
+    <t>Asteroid Lab</t>
+  </si>
+  <si>
+    <t>810102</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Postman Star Mock Service</t>
+  </si>
+  <si>
+    <t>NEW Postman Hospital 5</t>
+  </si>
+  <si>
+    <t>Codice L3</t>
+  </si>
+  <si>
+    <t>Codice L4</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,10 +179,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,153 +515,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Ospedale</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Laboratorio</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Codice L1</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Codice L2</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Codice Applicativo</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Nome applicativo</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Nome Collection Postman</v>
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Postman Space Hospital</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Comet Lab</v>
-      </c>
-      <c r="C2" t="str">
-        <v>309672</v>
-      </c>
-      <c r="D2" t="str">
-        <v>1234</v>
-      </c>
-      <c r="E2" t="str">
-        <v>1</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Postman Sun Mock Service</v>
-      </c>
-      <c r="G2" t="str">
-        <v xml:space="preserve">NEW Postman Hospital 1 </v>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Postman Space Hospital</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Nova Lab</v>
-      </c>
-      <c r="C3" t="str">
-        <v>309672</v>
-      </c>
-      <c r="D3" t="str">
-        <v>0912</v>
-      </c>
-      <c r="E3" t="str">
-        <v>2</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Postman Sky Mock Service</v>
-      </c>
-      <c r="G3" t="str">
-        <v>NEW Postman Hospital 2</v>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Postman Galaxy Hospital</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Orbit Lab</v>
-      </c>
-      <c r="C4" t="str">
-        <v>462801</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1996</v>
-      </c>
-      <c r="E4" t="str">
-        <v>3</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Postman Moon Mock Service</v>
-      </c>
-      <c r="G4" t="str">
-        <v>NEW Postman Hospital 3</v>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Postman Galaxy Hospital</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Nebula Lab</v>
-      </c>
-      <c r="C5" t="str">
-        <v>462801</v>
-      </c>
-      <c r="D5" t="str">
-        <v>5678</v>
-      </c>
-      <c r="E5" t="str">
-        <v>4</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Postman Milky Mock Service</v>
-      </c>
-      <c r="G5" t="str">
-        <v>NEW Postman Hospital 4</v>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Postman Cosmo Hospital</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Asteroid Lab</v>
-      </c>
-      <c r="C6" t="str">
-        <v>810102</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2014</v>
-      </c>
-      <c r="E6" t="str">
-        <v>5</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Postman Star Mock Service</v>
-      </c>
-      <c r="G6" t="str">
-        <v>NEW Postman Hospital 5</v>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError sqref="G1:I6 A1:D6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code updated with new profiles and support to L3 and L4 codes
</commit_message>
<xml_diff>
--- a/CensimentoEnti.xlsx
+++ b/CensimentoEnti.xlsx
@@ -1,41 +1,158 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.dileo\Documents\Python3\PostmanHospital\Postman-Hospital-Py\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB965B81-F79A-4033-ADE9-C3EB8C7EC1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+  <si>
+    <t>Ospedale</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Codice L1</t>
+  </si>
+  <si>
+    <t>Codice L2</t>
+  </si>
+  <si>
+    <t>Codice L3</t>
+  </si>
+  <si>
+    <t>Codice L4</t>
+  </si>
+  <si>
+    <t>Codice Applicativo</t>
+  </si>
+  <si>
+    <t>Nome applicativo</t>
+  </si>
+  <si>
+    <t>Nome Collection Postman</t>
+  </si>
+  <si>
+    <t>Postman Space Hospital</t>
+  </si>
+  <si>
+    <t>Comet Lab</t>
+  </si>
+  <si>
+    <t>309672</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Postman Sun Mock Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postman Hospital 1 </t>
+  </si>
+  <si>
+    <t>Nova Lab</t>
+  </si>
+  <si>
+    <t>0912</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Postman Sky Mock Service</t>
+  </si>
+  <si>
+    <t>Postman Hospital 2</t>
+  </si>
+  <si>
+    <t>Postman Galaxy Hospital</t>
+  </si>
+  <si>
+    <t>Orbit Lab</t>
+  </si>
+  <si>
+    <t>462801</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Postman Moon Mock Service</t>
+  </si>
+  <si>
+    <t>Postman Hospital 3</t>
+  </si>
+  <si>
+    <t>Nebula Lab</t>
+  </si>
+  <si>
+    <t>5678</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Postman Milky Mock Service</t>
+  </si>
+  <si>
+    <t>Postman Hospital 4</t>
+  </si>
+  <si>
+    <t>Postman Cosmo Hospital</t>
+  </si>
+  <si>
+    <t>Asteroid Lab</t>
+  </si>
+  <si>
+    <t>810102</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Postman Star Mock Service</t>
+  </si>
+  <si>
+    <t>Postman Hospital 5</t>
+  </si>
+  <si>
+    <t>0801</t>
+  </si>
+  <si>
+    <t>0913</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,14 +181,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,189 +530,202 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.796875" style="1"/>
+    <col min="7" max="7" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Ospedale</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Laboratorio</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Codice L1</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Codice L2</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Codice L3</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Codice L4</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Codice Applicativo</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Nome applicativo</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Nome Collection Postman</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Postman Space Hospital</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Comet Lab</v>
-      </c>
-      <c r="C2" t="str">
-        <v>309672</v>
-      </c>
-      <c r="D2" t="str">
-        <v>1234</v>
-      </c>
-      <c r="E2" t="str">
-        <v>309672</v>
-      </c>
-      <c r="F2" t="str">
-        <v>1234</v>
-      </c>
-      <c r="G2" t="str">
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Postman Sun Mock Service</v>
-      </c>
-      <c r="I2" t="str">
-        <v xml:space="preserve">Postman Hospital 1 </v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3">
+        <v>121314</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Postman Space Hospital</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Nova Lab</v>
-      </c>
-      <c r="C3" t="str">
-        <v>309672</v>
-      </c>
-      <c r="D3" t="str">
-        <v>0912</v>
-      </c>
-      <c r="E3" t="str">
-        <v>309672</v>
-      </c>
-      <c r="F3" t="str">
-        <v>0912</v>
-      </c>
-      <c r="G3" t="str">
-        <v>2</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Postman Sky Mock Service</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Postman Hospital 2</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3">
+        <v>129981</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Postman Galaxy Hospital</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Orbit Lab</v>
-      </c>
-      <c r="C4" t="str">
-        <v>462801</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1996</v>
-      </c>
-      <c r="E4" t="str">
-        <v>462801</v>
-      </c>
-      <c r="F4" t="str">
-        <v>1996</v>
-      </c>
-      <c r="G4" t="str">
-        <v>3</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Postman Moon Mock Service</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Postman Hospital 3</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7281</v>
+      </c>
+      <c r="F4" s="3">
+        <v>993932</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Postman Galaxy Hospital</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Nebula Lab</v>
-      </c>
-      <c r="C5" t="str">
-        <v>462801</v>
-      </c>
-      <c r="D5" t="str">
-        <v>5678</v>
-      </c>
-      <c r="E5" t="str">
-        <v>462801</v>
-      </c>
-      <c r="F5" t="str">
-        <v>5678</v>
-      </c>
-      <c r="G5" t="str">
-        <v>4</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Postman Milky Mock Service</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Postman Hospital 4</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1928</v>
+      </c>
+      <c r="F5" s="3">
+        <v>929292</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Postman Cosmo Hospital</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Asteroid Lab</v>
-      </c>
-      <c r="C6" t="str">
-        <v>810102</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2014</v>
-      </c>
-      <c r="E6" t="str">
-        <v>810102</v>
-      </c>
-      <c r="F6" t="str">
-        <v>2014</v>
-      </c>
-      <c r="G6" t="str">
-        <v>5</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Postman Star Mock Service</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Postman Hospital 5</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2991</v>
+      </c>
+      <c r="F6" s="3">
+        <v>237485</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
+    <ignoredError sqref="A1:I1 A2:D6 G2:I6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All functionalities tested and working (on 1 Req msgs) after huge OMR modifications
</commit_message>
<xml_diff>
--- a/CensimentoEnti.xlsx
+++ b/CensimentoEnti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.dileo\Documents\Python3\PostmanHospital\Postman-Hospital-Py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB965B81-F79A-4033-ADE9-C3EB8C7EC1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA7F760-C75F-45EA-992D-E747D85CC053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Ospedale</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Postman Sun Mock Service</t>
   </si>
   <si>
-    <t xml:space="preserve">Postman Hospital 1 </t>
-  </si>
-  <si>
     <t>Nova Lab</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Postman Sky Mock Service</t>
   </si>
   <si>
-    <t>Postman Hospital 2</t>
-  </si>
-  <si>
     <t>Postman Galaxy Hospital</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>Postman Moon Mock Service</t>
   </si>
   <si>
-    <t>Postman Hospital 3</t>
-  </si>
-  <si>
     <t>Nebula Lab</t>
   </si>
   <si>
@@ -118,9 +109,6 @@
     <t>Postman Milky Mock Service</t>
   </si>
   <si>
-    <t>Postman Hospital 4</t>
-  </si>
-  <si>
     <t>Postman Cosmo Hospital</t>
   </si>
   <si>
@@ -139,23 +127,44 @@
     <t>Postman Star Mock Service</t>
   </si>
   <si>
-    <t>Postman Hospital 5</t>
-  </si>
-  <si>
     <t>0801</t>
   </si>
   <si>
     <t>0913</t>
+  </si>
+  <si>
+    <t>Codice Laboratorio OMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postman Hospital Lab 1 </t>
+  </si>
+  <si>
+    <t>Postman Hospital Lab 2</t>
+  </si>
+  <si>
+    <t>Postman Hospital Lab 3</t>
+  </si>
+  <si>
+    <t>Postman Hospital Lab 4</t>
+  </si>
+  <si>
+    <t>Postman Hospital Lab 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -543,12 +552,12 @@
     <col min="2" max="2" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8.796875" style="1"/>
     <col min="7" max="7" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.796875" style="1"/>
+    <col min="8" max="9" width="25.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,13 +580,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -591,7 +603,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F2" s="3">
         <v>121314</v>
@@ -599,54 +611,60 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1">
+        <v>5072024</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
+      <c r="J2" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3">
         <v>129981</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5072025</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E4" s="1">
         <v>7281</v>
@@ -655,27 +673,30 @@
         <v>993932</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5072026</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="1">
         <v>1928</v>
@@ -684,27 +705,30 @@
         <v>929292</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5072027</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E6" s="1">
         <v>2991</v>
@@ -713,19 +737,23 @@
         <v>237485</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5072028</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I1 A2:D6 G2:I6" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:D6 I1:J1 G2:G6 A1:G1 I3:I6 I2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>